<commit_message>
only show not closed project
</commit_message>
<xml_diff>
--- a/NPI_Tracking.xlsx
+++ b/NPI_Tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bixingjian/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bixingjian/Documents/code/NPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57CAED1-6848-D643-8ECF-504E325DFF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EDA2FD-0859-7849-9D1E-EF19D5C39BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{0B907F6E-F2D6-8F4E-AB21-4517848A6D15}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{0B907F6E-F2D6-8F4E-AB21-4517848A6D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="51">
   <si>
     <t>S.NO</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Zon</t>
+  </si>
+  <si>
+    <t>someone</t>
+  </si>
+  <si>
+    <t>action itemenergy aasdfas for cindy 4</t>
+  </si>
+  <si>
+    <t>HVS 1BC 2</t>
   </si>
 </sst>
 </file>
@@ -535,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20D2F3E-4B46-7B48-B972-D6B84E6E20BC}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X5" sqref="A1:X5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,7 +684,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -1111,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C7F5EC-7B8C-9443-8E9E-1AFB9CD38FB4}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X5" sqref="T5:X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1260,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -1342,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -1369,7 +1378,7 @@
         <v>45446</v>
       </c>
       <c r="M5" s="1">
-        <v>45504</v>
+        <v>45492</v>
       </c>
       <c r="O5" s="1">
         <v>45687</v>
@@ -1387,7 +1396,7 @@
         <v>39</v>
       </c>
       <c r="W5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>